<commit_message>
Loading all tables complete
</commit_message>
<xml_diff>
--- a/test/data/TestExcelHelloComputer.xlsx
+++ b/test/data/TestExcelHelloComputer.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/borrellguillem/genai/hellocomputer/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3F5C06B-241B-E341-9B10-7118579BD695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A008CE-2A92-6347-89C9-F8CF009299FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21400" activeTab="1" xr2:uid="{A328486E-A4E2-414A-9663-B0F979980D8A}"/>
   </bookViews>
@@ -60,10 +60,10 @@
     <t>Question2</t>
   </si>
   <si>
-    <t>This table contains the results of of an exam. The first row contains the index for the questions, and the following column contains the answer to each question for each student. 1 means they provided the right answer, 0 means they provided the wrong answer</t>
-  </si>
-  <si>
     <t>answers</t>
+  </si>
+  <si>
+    <t>answers table contains the results of of an exam. The first row contains the index for the questions, and the following column contains the answer to each question for each student. 1 means they provided the right answer, 0 means they provided the wrong answer</t>
   </si>
 </sst>
 </file>
@@ -99,8 +99,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,29 +489,29 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
-    <col min="2" max="2" width="55.5" customWidth="1"/>
+    <col min="2" max="2" width="55.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>8</v>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="85" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
It works for the first template. V0.1
</commit_message>
<xml_diff>
--- a/test/data/TestExcelHelloComputer.xlsx
+++ b/test/data/TestExcelHelloComputer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/borrellguillem/genai/hellocomputer/test/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54A008CE-2A92-6347-89C9-F8CF009299FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C19401B-31D5-D842-B637-DE23C8761F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21400" activeTab="1" xr2:uid="{A328486E-A4E2-414A-9663-B0F979980D8A}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>Description</t>
   </si>
@@ -54,16 +54,25 @@
     <t>Question</t>
   </si>
   <si>
-    <t>Question1</t>
-  </si>
-  <si>
-    <t>Question2</t>
-  </si>
-  <si>
     <t>answers</t>
   </si>
   <si>
-    <t>answers table contains the results of of an exam. The first row contains the index for the questions, and the following column contains the answer to each question for each student. 1 means they provided the right answer, 0 means they provided the wrong answer</t>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Question 1</t>
+  </si>
+  <si>
+    <t>Question 2</t>
+  </si>
+  <si>
+    <t>Question 3</t>
+  </si>
+  <si>
+    <t>answers table contains the results of of an exam. The first row contains the question, the second contains the student name, and the third one contains the result for each question. 1 means they provided the right answer, 0 means they provided the wrong answer</t>
   </si>
 </sst>
 </file>
@@ -438,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B44CC28-8430-794C-868E-B252324107E5}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -451,18 +460,18 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -470,13 +479,57 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
       </c>
       <c r="C3">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -489,7 +542,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -503,7 +556,7 @@
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="85" x14ac:dyDescent="0.2">
@@ -511,7 +564,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>